<commit_message>
Atualização automática de SARANDI.xlsx
</commit_message>
<xml_diff>
--- a/SARANDI.xlsx
+++ b/SARANDI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C0A5DDA-AE59-422E-A96F-7051D115EC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EA5F114-3CA1-47CB-86B8-02CE78ADAF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1213,7 +1213,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{25C7CEC7-A144-43FC-962F-5B492BBDDF61}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{547B9C3D-EE7C-462B-A0A4-25E9AC414555}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1243,10 +1243,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E812A2F8-694A-4AAB-B63A-9440262102F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886A5D93-A497-4D43-9C0B-1BAFC192B7E1}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1284,7 +1284,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB4290B7-86D3-43BE-A905-F835E3E53C56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43DA96BF-9534-4562-A83C-398C430F6477}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1347,7 +1347,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B22F917-9AB0-4C3D-AB53-F6F1BC19F599}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7148837-6530-46F5-9D11-7D3F107984B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1366,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD1B2382-6763-45EA-EDA7-3EE5AAE0C226}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1122C58-1DBD-0F20-E54E-4DC15AADFCEC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1415,7 +1415,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D877ACD-F65C-186A-88B5-FC46224011C1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{913A2A13-A114-082B-C028-F91DCA39F71E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1434,7 +1434,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14DCE32F-7258-9B2E-4473-C775ED72C8BB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{814269F9-9D5F-0369-B597-65C10F41FD91}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1465,7 +1465,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67B561F0-37AB-8E80-DAD3-3EFE3529AD40}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{190F54BF-8786-5E82-0570-86106652F6DF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1496,7 +1496,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48EED127-0811-BC2C-78F2-2C5E7BE43BA6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C6BB45-A2A4-92FD-E18C-97E3BD5D4193}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1539,7 +1539,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B12D86C-A46C-4AE4-B0F1-A7C4E3D216BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2072B07-53DB-4086-934F-075371819E95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1577,7 +1577,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF38998D-528D-4FB1-8812-0821AAA17E90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37BCCD83-6E5D-47A2-81F4-50A537BC62D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1620,7 +1620,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D43F0CA-5F4B-40A8-9FFC-64DA068ECD61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00530B9F-2D6F-4BC1-9CC5-ED660BC6BDAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1933,7 +1933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A896D91-F70A-45DB-A689-0E8036113E66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A08FF1-86CD-4742-9120-2294D10690FA}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>